<commit_message>
changed for running our app in gcp
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elado\Desktop\University\Second\Preparatory Year\Semester A\IR\ProjectGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735CC8A2-F1F1-41F5-AE97-70381744A8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0A80F4-DAA0-49AC-A75D-92E2DEC42F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Quality</t>
   </si>
@@ -36,7 +36,13 @@
     <t>tf-idf, stemming, no lowering, wrong parsing, no stop words</t>
   </si>
   <si>
-    <t>tf-idf, stopwords, title 0.6, text 0.4, +pageranks 0.3</t>
+    <t>tf-idf, stopwords, title 0.55, text 0.45, +pageranks 0.3</t>
+  </si>
+  <si>
+    <t>tf-idf, stopwords, title 0.4, text 0.3, anchor 0.3 +pageranks 0.3</t>
+  </si>
+  <si>
+    <t>tf-idf, stopwords, title 0.4, text 0.2, anchor 0.4 +pageranks 0.3</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -395,6 +401,28 @@
         <v>22.629743448893201</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0.21790000000000001</v>
+      </c>
+      <c r="C16">
+        <v>19.803621347745199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0.21856666666666599</v>
+      </c>
+      <c r="C17">
+        <v>19.929215892155899</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding stop words and adding performances
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenan\Documents\לימודים\תשפד\סמסטר ה\אחזור מידע\פרוייקט\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE29F9F7-2E30-4CFE-B81B-7AD50F634DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3197737-399F-45F7-82CD-EF27DD41DDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Quality</t>
   </si>
@@ -118,6 +118,21 @@
   </si>
   <si>
     <t>tf-idf, stop words, title 0.55, text 0.35, anchor 0.1 +pagerank 0.35 no disambiguation pages, collect all docs of query in one list</t>
+  </si>
+  <si>
+    <t>tf-idf, stop words, title 0.6, text 0.3, anchor 0.1  no disambiguation pages, collect all docs of query in one list</t>
+  </si>
+  <si>
+    <t>tf-idf, stop words, title 0.6, text 0.3, anchor 0.1  +pagerank 0.5 no disambiguation pages, collect all docs of query in one list, query expansion 2 no duplicates</t>
+  </si>
+  <si>
+    <t>tf-idf, stop words, title 0.7, text 0.2, anchor 0.1   +pagerank 0.2 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list</t>
+  </si>
+  <si>
+    <t>tf-idf, stop words, title 0.7, text 0.2, anchor 0.1   +pagerank 0.2 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list, skip short docs (&gt;0.8)</t>
+  </si>
+  <si>
+    <t>tf-idf, stop words, title 0.6, text 0.3, anchor 0.1   +pagerank 0.4 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list, skip short docs (&gt;0.8)</t>
   </si>
 </sst>
 </file>
@@ -435,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="111.54296875" customWidth="1"/>
+    <col min="1" max="1" width="147.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -764,6 +779,61 @@
         <v>26.57</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>0.23043</v>
+      </c>
+      <c r="C31">
+        <v>21.61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>0.18060000000000001</v>
+      </c>
+      <c r="C32">
+        <v>38.598999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>0.21176</v>
+      </c>
+      <c r="C33">
+        <v>18.739000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>0.22539999999999999</v>
+      </c>
+      <c r="C34">
+        <v>9.7047000000000008</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>0.2437</v>
+      </c>
+      <c r="C35">
+        <v>20.9025</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
better results + adding performances
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenan\Documents\לימודים\תשפד\סמסטר ה\אחזור מידע\פרוייקט\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3197737-399F-45F7-82CD-EF27DD41DDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9560C3B1-F9CD-479C-B68D-30E10A8D8B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Quality</t>
   </si>
@@ -129,10 +129,13 @@
     <t>tf-idf, stop words, title 0.7, text 0.2, anchor 0.1   +pagerank 0.2 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list</t>
   </si>
   <si>
-    <t>tf-idf, stop words, title 0.7, text 0.2, anchor 0.1   +pagerank 0.2 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list, skip short docs (&gt;0.8)</t>
-  </si>
-  <si>
-    <t>tf-idf, stop words, title 0.6, text 0.3, anchor 0.1   +pagerank 0.4 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list, skip short docs (&gt;0.8)</t>
+    <t>tf-idf, stop words, title 0.7, text 0.2, anchor 0.1   +pagerank 0.2 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list, skip short docs (&gt;0.8), add stop words</t>
+  </si>
+  <si>
+    <t>tf-idf, stop words, title 0.6, text 0.3, anchor 0.1   +pagerank 0.4 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list, skip short docs (&gt;0.8), add stop words</t>
+  </si>
+  <si>
+    <t>tf-idf, stop words, title 0.6, text 0.3, anchor 0.1   +pagerank 0.4 no disambiguation pages, with anchor disambiguation, collect all docs of query in one list, skip short docs (&gt;0.7), add stop words</t>
   </si>
 </sst>
 </file>
@@ -450,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="147.54296875" customWidth="1"/>
+    <col min="1" max="1" width="178.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -834,6 +837,17 @@
         <v>20.9025</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>0.24673</v>
+      </c>
+      <c r="C36">
+        <v>14.43657</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>